<commit_message>
Minor Adjustment + added NashTech Area PeopleController
</commit_message>
<xml_diff>
--- a/Assignments/MVCDotNetAssignment/MVCDotNetAssignment.WebApp/wwwroot/ExportedFiles/People.xlsx
+++ b/Assignments/MVCDotNetAssignment/MVCDotNetAssignment.WebApp/wwwroot/ExportedFiles/People.xlsx
@@ -16,28 +16,28 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:si>
-    <x:t>First Name</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Last Name</x:t>
+    <x:t>FirstName</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LastName</x:t>
   </x:si>
   <x:si>
     <x:t>Gender</x:t>
   </x:si>
   <x:si>
-    <x:t>Date of Birth</x:t>
+    <x:t>DoB</x:t>
   </x:si>
   <x:si>
     <x:t>Birthplace</x:t>
   </x:si>
   <x:si>
-    <x:t>Phone Number</x:t>
+    <x:t>PhoneNumber</x:t>
   </x:si>
   <x:si>
     <x:t>Age</x:t>
   </x:si>
   <x:si>
-    <x:t>Is Graduated</x:t>
+    <x:t>IsGraduated</x:t>
   </x:si>
   <x:si>
     <x:t>Ánh</x:t>

</xml_diff>